<commit_message>
final mentors list linked to mongo
</commit_message>
<xml_diff>
--- a/backend/Final XSEED Mentor List.xlsx
+++ b/backend/Final XSEED Mentor List.xlsx
@@ -1612,7 +1612,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>27</v>
@@ -1668,7 +1668,7 @@
         <v>26</v>
       </c>
       <c r="L3" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>38</v>
@@ -1724,7 +1724,7 @@
         <v>49</v>
       </c>
       <c r="L4" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>50</v>
@@ -1780,7 +1780,7 @@
         <v>26</v>
       </c>
       <c r="L5" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>61</v>
@@ -1836,7 +1836,7 @@
         <v>26</v>
       </c>
       <c r="L6" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>72</v>
@@ -1892,7 +1892,7 @@
         <v>26</v>
       </c>
       <c r="L7" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>81</v>
@@ -1948,7 +1948,7 @@
         <v>91</v>
       </c>
       <c r="L8" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>92</v>
@@ -2004,7 +2004,7 @@
         <v>26</v>
       </c>
       <c r="L9" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>102</v>
@@ -2060,7 +2060,7 @@
         <v>26</v>
       </c>
       <c r="L10" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>112</v>
@@ -2116,7 +2116,7 @@
         <v>49</v>
       </c>
       <c r="L11" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>121</v>
@@ -2172,7 +2172,7 @@
         <v>49</v>
       </c>
       <c r="L12" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>130</v>
@@ -2228,7 +2228,7 @@
         <v>26</v>
       </c>
       <c r="L13" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>139</v>
@@ -2284,7 +2284,7 @@
         <v>26</v>
       </c>
       <c r="L14" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>147</v>
@@ -2340,7 +2340,7 @@
         <v>49</v>
       </c>
       <c r="L15" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>157</v>
@@ -2396,7 +2396,7 @@
         <v>26</v>
       </c>
       <c r="L16" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>165</v>
@@ -2452,7 +2452,7 @@
         <v>26</v>
       </c>
       <c r="L17" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M17" s="3" t="s">
         <v>174</v>
@@ -2508,7 +2508,7 @@
         <v>49</v>
       </c>
       <c r="L18" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>183</v>
@@ -2564,7 +2564,7 @@
         <v>26</v>
       </c>
       <c r="L19" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M19" s="3" t="s">
         <v>192</v>
@@ -2620,7 +2620,7 @@
         <v>26</v>
       </c>
       <c r="L20" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>202</v>
@@ -2676,7 +2676,7 @@
         <v>26</v>
       </c>
       <c r="L21" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M21" s="3" t="s">
         <v>121</v>
@@ -2732,7 +2732,7 @@
         <v>26</v>
       </c>
       <c r="L22" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>212</v>
@@ -2788,7 +2788,7 @@
         <v>26</v>
       </c>
       <c r="L23" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>221</v>
@@ -2844,7 +2844,7 @@
         <v>26</v>
       </c>
       <c r="L24" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>139</v>
@@ -2900,7 +2900,7 @@
         <v>49</v>
       </c>
       <c r="L25" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>233</v>
@@ -2956,7 +2956,7 @@
         <v>26</v>
       </c>
       <c r="L26" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>243</v>
@@ -3012,7 +3012,7 @@
         <v>26</v>
       </c>
       <c r="L27" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>251</v>
@@ -3068,7 +3068,7 @@
         <v>26</v>
       </c>
       <c r="L28" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>260</v>
@@ -3124,7 +3124,7 @@
         <v>49</v>
       </c>
       <c r="L29" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M29" s="3" t="s">
         <v>269</v>
@@ -3180,7 +3180,7 @@
         <v>26</v>
       </c>
       <c r="L30" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>278</v>
@@ -3236,7 +3236,7 @@
         <v>91</v>
       </c>
       <c r="L31" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>287</v>
@@ -3292,7 +3292,7 @@
         <v>26</v>
       </c>
       <c r="L32" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M32" s="3" t="s">
         <v>294</v>
@@ -3348,7 +3348,7 @@
         <v>26</v>
       </c>
       <c r="L33" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M33" s="3" t="s">
         <v>302</v>
@@ -3404,7 +3404,7 @@
         <v>26</v>
       </c>
       <c r="L34" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>310</v>
@@ -3460,7 +3460,7 @@
         <v>49</v>
       </c>
       <c r="L35" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M35" s="3" t="s">
         <v>318</v>
@@ -3516,7 +3516,7 @@
         <v>49</v>
       </c>
       <c r="L36" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M36" s="3" t="s">
         <v>326</v>
@@ -3572,7 +3572,7 @@
         <v>26</v>
       </c>
       <c r="L37" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M37" s="3" t="s">
         <v>333</v>
@@ -3628,7 +3628,7 @@
         <v>26</v>
       </c>
       <c r="L38" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M38" s="3" t="s">
         <v>341</v>
@@ -3684,7 +3684,7 @@
         <v>49</v>
       </c>
       <c r="L39" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>348</v>
@@ -3740,7 +3740,7 @@
         <v>26</v>
       </c>
       <c r="L40" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M40" s="3" t="s">
         <v>357</v>
@@ -3796,7 +3796,7 @@
         <v>26</v>
       </c>
       <c r="L41" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M41" s="3" t="s">
         <v>364</v>
@@ -3852,7 +3852,7 @@
         <v>26</v>
       </c>
       <c r="L42" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>372</v>
@@ -3908,7 +3908,7 @@
         <v>26</v>
       </c>
       <c r="L43" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M43" s="3" t="s">
         <v>379</v>
@@ -3964,7 +3964,7 @@
         <v>91</v>
       </c>
       <c r="L44" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>387</v>
@@ -4020,7 +4020,7 @@
         <v>26</v>
       </c>
       <c r="L45" s="2">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>396</v>

</xml_diff>